<commit_message>
test 24, 25, 26
</commit_message>
<xml_diff>
--- a/JPS_1_AST/misc/Zapytania testowe JPS.xlsx
+++ b/JPS_1_AST/misc/Zapytania testowe JPS.xlsx
@@ -962,7 +962,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1159,7 +1159,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
zaimplementowane asserty we wszystkich nowych testcase'ach
</commit_message>
<xml_diff>
--- a/JPS_1_AST/misc/Zapytania testowe JPS.xlsx
+++ b/JPS_1_AST/misc/Zapytania testowe JPS.xlsx
@@ -640,14 +640,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,9 +952,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -975,7 +975,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="b">
+      <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -983,7 +983,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="b">
+      <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="b">
+      <c r="B4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -999,7 +999,7 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="b">
+      <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="b">
+      <c r="B6" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="b">
+      <c r="B7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1023,15 +1023,15 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="b">
+      <c r="B9" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="b">
+      <c r="B10" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>192</v>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>193</v>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       <c r="A32" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       <c r="A34" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       <c r="A35" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="3" t="b">
+      <c r="B35" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="3" t="b">
+      <c r="B36" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       <c r="A37" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       <c r="A38" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="3" t="b">
+      <c r="B38" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="3" t="b">
+      <c r="B39" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="3" t="b">
+      <c r="B40" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       <c r="A41" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="3" t="b">
+      <c r="B41" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="3" t="b">
+      <c r="B42" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="3" t="b">
+      <c r="B43" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="3" t="b">
+      <c r="B44" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       <c r="A45" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="3" t="b">
+      <c r="B45" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       <c r="A46" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="3" t="b">
+      <c r="B46" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="3" t="b">
+      <c r="B47" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       <c r="A48" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="3" t="b">
+      <c r="B48" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       <c r="A49" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       <c r="A50" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       <c r="A51" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       <c r="A52" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1383,7 +1383,7 @@
       <c r="A53" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       <c r="A54" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       <c r="A55" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
       <c r="A56" t="s">
         <v>79</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       <c r="A57" t="s">
         <v>80</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="A60" t="s">
         <v>86</v>
       </c>
-      <c r="B60" t="b">
+      <c r="B60" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       <c r="A61" t="s">
         <v>87</v>
       </c>
-      <c r="B61" t="b">
+      <c r="B61" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       <c r="A62" t="s">
         <v>88</v>
       </c>
-      <c r="B62" t="b">
+      <c r="B62" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       <c r="A63" t="s">
         <v>89</v>
       </c>
-      <c r="B63" t="b">
+      <c r="B63" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       <c r="A64" t="s">
         <v>90</v>
       </c>
-      <c r="B64" t="b">
+      <c r="B64" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       <c r="A65" t="s">
         <v>91</v>
       </c>
-      <c r="B65" t="b">
+      <c r="B65" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       <c r="A66" t="s">
         <v>92</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       <c r="A67" t="s">
         <v>93</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
       <c r="A68" t="s">
         <v>95</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       <c r="A69" t="s">
         <v>96</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
       <c r="A70" t="s">
         <v>98</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       <c r="A71" t="s">
         <v>100</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       <c r="A72" t="s">
         <v>102</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
       <c r="A73" t="s">
         <v>104</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       <c r="A74" t="s">
         <v>106</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       <c r="A75" t="s">
         <v>108</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="A76" t="s">
         <v>110</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1575,7 +1575,7 @@
       <c r="A77" t="s">
         <v>112</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       <c r="A78" t="s">
         <v>113</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       <c r="A79" t="s">
         <v>115</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       <c r="A80" t="s">
         <v>117</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       <c r="A81" t="s">
         <v>118</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       <c r="A82" t="s">
         <v>120</v>
       </c>
-      <c r="B82" t="b">
+      <c r="B82" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       <c r="A83" t="s">
         <v>121</v>
       </c>
-      <c r="B83" t="b">
+      <c r="B83" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       <c r="A84" t="s">
         <v>122</v>
       </c>
-      <c r="B84" t="b">
+      <c r="B84" s="2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       <c r="A85" t="s">
         <v>123</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       <c r="A86" t="s">
         <v>125</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       <c r="A87" t="s">
         <v>127</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       <c r="A88" t="s">
         <v>128</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
       <c r="A89" t="s">
         <v>130</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       <c r="A90" t="s">
         <v>132</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       <c r="A91" t="s">
         <v>134</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       <c r="A92" t="s">
         <v>136</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="2" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       <c r="A93" t="s">
         <v>138</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
       <c r="A94" t="s">
         <v>139</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       <c r="A95" t="s">
         <v>140</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       <c r="A96" t="s">
         <v>142</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
       <c r="A97" t="s">
         <v>143</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1743,7 +1743,7 @@
       <c r="A98" t="s">
         <v>145</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       <c r="A99" t="s">
         <v>147</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       <c r="A100" t="s">
         <v>149</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
       <c r="A101" t="s">
         <v>150</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
       <c r="A102" t="s">
         <v>152</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
       <c r="A103" t="s">
         <v>153</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="2" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       <c r="A105" t="s">
         <v>157</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       <c r="A106" t="s">
         <v>158</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       <c r="A107" t="s">
         <v>160</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1823,7 +1823,7 @@
       <c r="A108" t="s">
         <v>161</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="2" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
       <c r="A109" t="s">
         <v>163</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       <c r="A110" t="s">
         <v>164</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       <c r="A111" t="s">
         <v>166</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       <c r="A112" t="s">
         <v>167</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1863,7 +1863,7 @@
       <c r="A113" t="s">
         <v>169</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       <c r="A114" t="s">
         <v>170</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       <c r="A115" t="s">
         <v>171</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       <c r="A116" t="s">
         <v>172</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="A117" t="s">
         <v>173</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       <c r="A118" t="s">
         <v>174</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
       <c r="A119" t="s">
         <v>175</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       <c r="A120" t="s">
         <v>176</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       <c r="A121" t="s">
         <v>177</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
       <c r="A122" t="s">
         <v>178</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
       <c r="A123" t="s">
         <v>179</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       <c r="A124" t="s">
         <v>180</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       <c r="A125" t="s">
         <v>181</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       <c r="A126" t="s">
         <v>182</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
       <c r="A127" t="s">
         <v>183</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
       <c r="A128" t="s">
         <v>184</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       <c r="A129" t="s">
         <v>185</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
       <c r="A130" t="s">
         <v>186</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       <c r="A131" t="s">
         <v>187</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2015,7 +2015,7 @@
       <c r="A132" t="s">
         <v>188</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="2" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>